<commit_message>
Many analysis updates. Added "commonness" trait. Updated diet quality metric to be a nutrient density index Syntax files cleaned and re-dated to reflect current main analysis. All R files re-run and debugged All updated analysis is dated 20221104 Old syntax files archived
</commit_message>
<xml_diff>
--- a/output/20221101/wald_tests.xlsx
+++ b/output/20221101/wald_tests.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erb32/github/cambodia_biodiversity2/output/20221101/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4EBC63-2169-AD40-8FF9-09736A7C1175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDF93B2-5A6A-794C-93C6-BB2CCD53E960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500"/>
   </bookViews>
   <sheets>
     <sheet name="Species count models" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="22">
   <si>
     <t>Outcome</t>
   </si>
@@ -72,6 +72,33 @@
   </si>
   <si>
     <t>pval</t>
+  </si>
+  <si>
+    <t>Base = Effort</t>
+  </si>
+  <si>
+    <t>Effort = HH</t>
+  </si>
+  <si>
+    <t>HH = Market</t>
+  </si>
+  <si>
+    <t>Market = Market X</t>
+  </si>
+  <si>
+    <t>HH = Effort</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Includes effort control</t>
+  </si>
+  <si>
+    <t>No effort control</t>
   </si>
 </sst>
 </file>
@@ -84,21 +111,15 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -113,14 +134,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,21 +457,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="13.33203125" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="15" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="4.6640625" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -462,8 +484,11 @@
       <c r="D1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -473,11 +498,14 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <v>0.39359426498413086</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -487,11 +515,14 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <v>0.39513945579528809</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -501,11 +532,14 @@
       <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <v>0.45836341381072998</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -515,11 +549,14 @@
       <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <v>0.47120442986488342</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -529,11 +566,14 @@
       <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>0.7395748496055603</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -543,11 +583,14 @@
       <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="2">
         <v>0.95869630575180054</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -557,11 +600,14 @@
       <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="2">
         <v>0.49294984340667725</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -571,11 +617,14 @@
       <c r="C9" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="2">
         <v>0.99645304679870605</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -586,10 +635,13 @@
         <v>7</v>
       </c>
       <c r="D10" s="2">
-        <v>2.5289285928010941E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.025289285928010941</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -599,11 +651,14 @@
       <c r="C11" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="2">
         <v>0.60437321662902832</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -613,11 +668,14 @@
       <c r="C12" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="2">
         <v>0.38246056437492371</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -627,11 +685,14 @@
       <c r="C13" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="2">
         <v>0.95514136552810669</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -639,80 +700,234 @@
         <v>5</v>
       </c>
       <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.39704379439353943</v>
+      </c>
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.36156192421913147</v>
+      </c>
+      <c r="E15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.46074551343917847</v>
+      </c>
+      <c r="E16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.75055629014968872</v>
+      </c>
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.38944357633590698</v>
+      </c>
+      <c r="E18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.49287569522857666</v>
+      </c>
+      <c r="E19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.86214041709899902</v>
+      </c>
+      <c r="E20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.87446886301040649</v>
+      </c>
+      <c r="E21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D22" s="2">
         <v>0.7497296929359436</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="E22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D23" s="2">
         <v>0.46951273083686829</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="E23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D24" s="2">
         <v>0.166672483086586</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="E24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D25" s="2">
         <v>0.2576880156993866</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="E25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D26" s="2">
         <v>0.65705549716949463</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="E26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D27" s="2">
         <v>0.36478361487388611</v>
+      </c>
+      <c r="E27" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>